<commit_message>
deleted redundant file aact-data-definitions[old]
</commit_message>
<xml_diff>
--- a/public/documentation/aact_data_definitions.xlsx
+++ b/public/documentation/aact_data_definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariannademenko/ID/CTD/aact-admin/public/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02663339-BB3E-3545-8744-A15F1311B820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AC584D-36D5-F14D-BEC0-2F5BDB028E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AACT Tables and Columns" sheetId="1" r:id="rId1"/>
@@ -4342,8 +4342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1022"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A396" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="B400" sqref="B400"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>